<commit_message>
chore: clean restructure + updated docs
</commit_message>
<xml_diff>
--- a/data/raw/AI_Cost_Estimator_Catalog_UPDATED.xlsx
+++ b/data/raw/AI_Cost_Estimator_Catalog_UPDATED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shashank_work\Python_Works\AI_Hackathon_October_2025_v1_demo\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BBB2C0-EC32-4CD9-B60A-71B0EE46341A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5637E267-CC07-4BA2-AF1C-13CA8084248B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6360" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1443,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A186" sqref="A186"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
         <v>46</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -2793,7 +2793,7 @@
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
         <v>44</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="18" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
         <v>44</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="19" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
@@ -3238,7 +3238,7 @@
     </row>
     <row r="20" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
@@ -3327,7 +3327,7 @@
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>44</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
         <v>44</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="23" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
@@ -3594,7 +3594,7 @@
     </row>
     <row r="24" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
@@ -3778,7 +3778,7 @@
     </row>
     <row r="26" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
         <v>44</v>
@@ -3867,7 +3867,7 @@
     </row>
     <row r="27" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
         <v>44</v>
@@ -3956,7 +3956,7 @@
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
@@ -4045,7 +4045,7 @@
     </row>
     <row r="29" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
@@ -4134,7 +4134,7 @@
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
         <v>44</v>
@@ -4223,7 +4223,7 @@
     </row>
     <row r="31" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
         <v>44</v>
@@ -4312,7 +4312,7 @@
     </row>
     <row r="32" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
         <v>44</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
         <v>44</v>
@@ -4579,7 +4579,7 @@
     </row>
     <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
         <v>44</v>
@@ -4674,7 +4674,7 @@
     </row>
     <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>44</v>
@@ -4763,7 +4763,7 @@
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
         <v>44</v>
@@ -4852,7 +4852,7 @@
     </row>
     <row r="38" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
         <v>44</v>
@@ -4941,7 +4941,7 @@
     </row>
     <row r="39" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
         <v>44</v>
@@ -5030,7 +5030,7 @@
     </row>
     <row r="40" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
         <v>44</v>
@@ -5119,7 +5119,7 @@
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
         <v>44</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="42" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
         <v>44</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="43" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -5386,7 +5386,7 @@
     </row>
     <row r="44" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
         <v>44</v>
@@ -5475,7 +5475,7 @@
     </row>
     <row r="45" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
@@ -5570,7 +5570,7 @@
     </row>
     <row r="46" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
         <v>44</v>
@@ -5659,7 +5659,7 @@
     </row>
     <row r="47" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
         <v>44</v>
@@ -5748,7 +5748,7 @@
     </row>
     <row r="48" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B48" t="s">
         <v>44</v>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="49" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
         <v>44</v>
@@ -5926,7 +5926,7 @@
     </row>
     <row r="50" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
         <v>44</v>
@@ -6015,7 +6015,7 @@
     </row>
     <row r="51" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B51" t="s">
         <v>44</v>
@@ -6104,7 +6104,7 @@
     </row>
     <row r="52" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B52" t="s">
         <v>44</v>
@@ -6193,7 +6193,7 @@
     </row>
     <row r="53" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B53" t="s">
         <v>47</v>
@@ -6285,7 +6285,7 @@
     </row>
     <row r="54" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B54" t="s">
         <v>47</v>
@@ -6377,7 +6377,7 @@
     </row>
     <row r="55" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="B55" t="s">
         <v>47</v>
@@ -6469,7 +6469,7 @@
     </row>
     <row r="56" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B56" t="s">
         <v>47</v>
@@ -6561,7 +6561,7 @@
     </row>
     <row r="57" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B57" t="s">
         <v>47</v>
@@ -6653,7 +6653,7 @@
     </row>
     <row r="58" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
         <v>47</v>
@@ -6745,7 +6745,7 @@
     </row>
     <row r="59" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
         <v>47</v>
@@ -6837,7 +6837,7 @@
     </row>
     <row r="60" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
         <v>47</v>
@@ -6929,7 +6929,7 @@
     </row>
     <row r="61" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
         <v>44</v>
@@ -7024,7 +7024,7 @@
     </row>
     <row r="62" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B62" t="s">
         <v>47</v>
@@ -7116,7 +7116,7 @@
     </row>
     <row r="63" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B63" t="s">
         <v>47</v>
@@ -7208,7 +7208,7 @@
     </row>
     <row r="64" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B64" t="s">
         <v>47</v>
@@ -7300,7 +7300,7 @@
     </row>
     <row r="65" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B65" t="s">
         <v>47</v>
@@ -7392,7 +7392,7 @@
     </row>
     <row r="66" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
         <v>47</v>
@@ -7484,7 +7484,7 @@
     </row>
     <row r="67" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B67" t="s">
         <v>47</v>
@@ -7576,7 +7576,7 @@
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
         <v>47</v>
@@ -7668,7 +7668,7 @@
     </row>
     <row r="69" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B69" t="s">
         <v>47</v>
@@ -7760,7 +7760,7 @@
     </row>
     <row r="70" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B70" t="s">
         <v>47</v>
@@ -7855,7 +7855,7 @@
     </row>
     <row r="71" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B71" t="s">
         <v>47</v>
@@ -7950,7 +7950,7 @@
     </row>
     <row r="72" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B72" t="s">
         <v>47</v>
@@ -8045,7 +8045,7 @@
     </row>
     <row r="73" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B73" t="s">
         <v>47</v>
@@ -8140,7 +8140,7 @@
     </row>
     <row r="74" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B74" t="s">
         <v>47</v>
@@ -8235,7 +8235,7 @@
     </row>
     <row r="75" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="B75" t="s">
         <v>44</v>
@@ -8330,7 +8330,7 @@
     </row>
     <row r="76" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B76" t="s">
         <v>47</v>
@@ -8425,7 +8425,7 @@
     </row>
     <row r="77" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B77" t="s">
         <v>47</v>
@@ -8520,7 +8520,7 @@
     </row>
     <row r="78" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B78" t="s">
         <v>47</v>
@@ -8615,7 +8615,7 @@
     </row>
     <row r="79" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B79" t="s">
         <v>47</v>
@@ -8710,7 +8710,7 @@
     </row>
     <row r="80" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B80" t="s">
         <v>47</v>
@@ -8805,7 +8805,7 @@
     </row>
     <row r="81" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B81" t="s">
         <v>47</v>
@@ -8900,7 +8900,7 @@
     </row>
     <row r="82" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B82" t="s">
         <v>47</v>
@@ -8995,7 +8995,7 @@
     </row>
     <row r="83" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B83" t="s">
         <v>47</v>
@@ -9090,7 +9090,7 @@
     </row>
     <row r="84" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B84" t="s">
         <v>47</v>
@@ -9185,7 +9185,7 @@
     </row>
     <row r="85" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B85" t="s">
         <v>47</v>
@@ -9283,7 +9283,7 @@
     </row>
     <row r="86" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B86" t="s">
         <v>47</v>
@@ -9378,7 +9378,7 @@
     </row>
     <row r="87" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B87" t="s">
         <v>45</v>
@@ -9467,7 +9467,7 @@
     </row>
     <row r="88" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B88" t="s">
         <v>45</v>
@@ -9556,7 +9556,7 @@
     </row>
     <row r="89" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="B89" t="s">
         <v>45</v>
@@ -9645,7 +9645,7 @@
     </row>
     <row r="90" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B90" t="s">
         <v>45</v>
@@ -9734,7 +9734,7 @@
     </row>
     <row r="91" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="B91" t="s">
         <v>47</v>
@@ -9835,7 +9835,7 @@
     </row>
     <row r="92" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B92" t="s">
         <v>45</v>
@@ -9924,7 +9924,7 @@
     </row>
     <row r="93" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B93" t="s">
         <v>45</v>
@@ -10025,7 +10025,7 @@
     </row>
     <row r="94" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B94" t="s">
         <v>45</v>
@@ -10129,7 +10129,7 @@
     </row>
     <row r="95" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B95" t="s">
         <v>47</v>
@@ -10230,7 +10230,7 @@
     </row>
     <row r="96" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="B96" t="s">
         <v>45</v>
@@ -10319,7 +10319,7 @@
     </row>
     <row r="97" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B97" t="s">
         <v>45</v>
@@ -10408,7 +10408,7 @@
     </row>
     <row r="98" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="B98" t="s">
         <v>45</v>
@@ -10497,7 +10497,7 @@
     </row>
     <row r="99" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="B99" t="s">
         <v>45</v>
@@ -10586,7 +10586,7 @@
     </row>
     <row r="100" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="B100" t="s">
         <v>45</v>
@@ -10675,7 +10675,7 @@
     </row>
     <row r="101" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B101" t="s">
         <v>45</v>
@@ -10770,7 +10770,7 @@
     </row>
     <row r="102" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="B102" t="s">
         <v>45</v>
@@ -10859,7 +10859,7 @@
     </row>
     <row r="103" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B103" t="s">
         <v>45</v>
@@ -10960,7 +10960,7 @@
     </row>
     <row r="104" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B104" t="s">
         <v>45</v>
@@ -11049,7 +11049,7 @@
     </row>
     <row r="105" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B105" t="s">
         <v>45</v>
@@ -11144,7 +11144,7 @@
     </row>
     <row r="106" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B106" t="s">
         <v>45</v>
@@ -11233,7 +11233,7 @@
     </row>
     <row r="107" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B107" t="s">
         <v>45</v>
@@ -11322,7 +11322,7 @@
     </row>
     <row r="108" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B108" t="s">
         <v>45</v>
@@ -11411,7 +11411,7 @@
     </row>
     <row r="109" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B109" t="s">
         <v>45</v>
@@ -11500,7 +11500,7 @@
     </row>
     <row r="110" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B110" t="s">
         <v>45</v>
@@ -11589,7 +11589,7 @@
     </row>
     <row r="111" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="B111" t="s">
         <v>45</v>
@@ -11690,7 +11690,7 @@
     </row>
     <row r="112" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B112" t="s">
         <v>45</v>
@@ -11794,7 +11794,7 @@
     </row>
     <row r="113" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="B113" t="s">
         <v>45</v>
@@ -11889,7 +11889,7 @@
     </row>
     <row r="114" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B114" t="s">
         <v>45</v>
@@ -11978,7 +11978,7 @@
     </row>
     <row r="115" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B115" t="s">
         <v>45</v>
@@ -12073,7 +12073,7 @@
     </row>
     <row r="116" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B116" t="s">
         <v>45</v>
@@ -12162,7 +12162,7 @@
     </row>
     <row r="117" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="B117" t="s">
         <v>45</v>
@@ -12251,7 +12251,7 @@
     </row>
     <row r="118" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B118" t="s">
         <v>45</v>
@@ -12340,7 +12340,7 @@
     </row>
     <row r="119" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B119" t="s">
         <v>45</v>
@@ -12429,7 +12429,7 @@
     </row>
     <row r="120" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B120" t="s">
         <v>45</v>
@@ -12518,7 +12518,7 @@
     </row>
     <row r="121" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="B121" t="s">
         <v>46</v>
@@ -12607,7 +12607,7 @@
     </row>
     <row r="122" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>121</v>
+        <v>154</v>
       </c>
       <c r="B122" t="s">
         <v>46</v>
@@ -12696,7 +12696,7 @@
     </row>
     <row r="123" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="B123" t="s">
         <v>46</v>
@@ -12785,7 +12785,7 @@
     </row>
     <row r="124" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="B124" t="s">
         <v>46</v>
@@ -12892,7 +12892,7 @@
     </row>
     <row r="125" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="B125" t="s">
         <v>46</v>
@@ -12996,7 +12996,7 @@
     </row>
     <row r="126" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>125</v>
+        <v>166</v>
       </c>
       <c r="B126" t="s">
         <v>46</v>
@@ -13103,7 +13103,7 @@
     </row>
     <row r="127" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>126</v>
+        <v>159</v>
       </c>
       <c r="B127" t="s">
         <v>46</v>
@@ -13192,7 +13192,7 @@
     </row>
     <row r="128" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="B128" t="s">
         <v>46</v>
@@ -13281,7 +13281,7 @@
     </row>
     <row r="129" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>128</v>
+        <v>161</v>
       </c>
       <c r="B129" t="s">
         <v>46</v>
@@ -13370,7 +13370,7 @@
     </row>
     <row r="130" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="B130" t="s">
         <v>46</v>
@@ -13459,7 +13459,7 @@
     </row>
     <row r="131" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="B131" t="s">
         <v>46</v>
@@ -13548,7 +13548,7 @@
     </row>
     <row r="132" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="B132" t="s">
         <v>46</v>
@@ -13637,7 +13637,7 @@
     </row>
     <row r="133" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="B133" t="s">
         <v>46</v>
@@ -13726,7 +13726,7 @@
     </row>
     <row r="134" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B134" t="s">
         <v>46</v>
@@ -13821,7 +13821,7 @@
     </row>
     <row r="135" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="B135" t="s">
         <v>46</v>
@@ -13925,7 +13925,7 @@
     </row>
     <row r="136" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B136" t="s">
         <v>46</v>
@@ -14020,7 +14020,7 @@
     </row>
     <row r="137" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B137" t="s">
         <v>46</v>
@@ -14115,7 +14115,7 @@
     </row>
     <row r="138" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B138" t="s">
         <v>46</v>
@@ -14204,7 +14204,7 @@
     </row>
     <row r="139" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B139" t="s">
         <v>46</v>
@@ -14293,7 +14293,7 @@
     </row>
     <row r="140" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B140" t="s">
         <v>46</v>
@@ -14382,7 +14382,7 @@
     </row>
     <row r="141" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B141" t="s">
         <v>46</v>
@@ -14471,7 +14471,7 @@
     </row>
     <row r="142" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B142" t="s">
         <v>46</v>
@@ -14560,7 +14560,7 @@
     </row>
     <row r="143" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B143" t="s">
         <v>46</v>
@@ -14649,7 +14649,7 @@
     </row>
     <row r="144" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B144" t="s">
         <v>46</v>
@@ -14738,7 +14738,7 @@
     </row>
     <row r="145" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B145" t="s">
         <v>46</v>
@@ -14827,7 +14827,7 @@
     </row>
     <row r="146" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B146" t="s">
         <v>46</v>
@@ -14916,7 +14916,7 @@
     </row>
     <row r="147" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="B147" t="s">
         <v>48</v>
@@ -15014,7 +15014,7 @@
     </row>
     <row r="148" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B148" t="s">
         <v>46</v>
@@ -15103,7 +15103,7 @@
     </row>
     <row r="149" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B149" t="s">
         <v>46</v>
@@ -15192,7 +15192,7 @@
     </row>
     <row r="150" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B150" t="s">
         <v>46</v>
@@ -15281,7 +15281,7 @@
     </row>
     <row r="151" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B151" t="s">
         <v>46</v>
@@ -15370,7 +15370,7 @@
     </row>
     <row r="152" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B152" t="s">
         <v>46</v>
@@ -15459,7 +15459,7 @@
     </row>
     <row r="153" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="B153" t="s">
         <v>46</v>
@@ -15548,7 +15548,7 @@
     </row>
     <row r="154" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="B154" t="s">
         <v>46</v>
@@ -15637,7 +15637,7 @@
     </row>
     <row r="155" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="B155" t="s">
         <v>46</v>
@@ -15726,7 +15726,7 @@
     </row>
     <row r="156" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="B156" t="s">
         <v>46</v>
@@ -15815,7 +15815,7 @@
     </row>
     <row r="157" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="B157" t="s">
         <v>46</v>
@@ -15904,7 +15904,7 @@
     </row>
     <row r="158" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="B158" t="s">
         <v>46</v>
@@ -15993,7 +15993,7 @@
     </row>
     <row r="159" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="B159" t="s">
         <v>46</v>
@@ -16082,7 +16082,7 @@
     </row>
     <row r="160" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>159</v>
+        <v>36</v>
       </c>
       <c r="B160" t="s">
         <v>44</v>
@@ -16177,7 +16177,7 @@
     </row>
     <row r="161" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="B161" t="s">
         <v>46</v>
@@ -16266,7 +16266,7 @@
     </row>
     <row r="162" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="B162" t="s">
         <v>46</v>
@@ -16355,7 +16355,7 @@
     </row>
     <row r="163" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="B163" t="s">
         <v>46</v>
@@ -16444,7 +16444,7 @@
     </row>
     <row r="164" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="B164" t="s">
         <v>46</v>
@@ -16533,7 +16533,7 @@
     </row>
     <row r="165" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="B165" t="s">
         <v>46</v>
@@ -16622,7 +16622,7 @@
     </row>
     <row r="166" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B166" t="s">
         <v>46</v>
@@ -16711,7 +16711,7 @@
     </row>
     <row r="167" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="B167" t="s">
         <v>46</v>
@@ -16800,7 +16800,7 @@
     </row>
     <row r="168" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="B168" t="s">
         <v>46</v>
@@ -16889,7 +16889,7 @@
     </row>
     <row r="169" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="B169" t="s">
         <v>46</v>
@@ -16978,7 +16978,7 @@
     </row>
     <row r="170" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="B170" t="s">
         <v>48</v>
@@ -17070,7 +17070,7 @@
     </row>
     <row r="171" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="B171" t="s">
         <v>48</v>
@@ -17162,7 +17162,7 @@
     </row>
     <row r="172" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B172" t="s">
         <v>48</v>
@@ -17254,7 +17254,7 @@
     </row>
     <row r="173" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="B173" t="s">
         <v>48</v>
@@ -17346,7 +17346,7 @@
     </row>
     <row r="174" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="B174" t="s">
         <v>48</v>
@@ -17438,7 +17438,7 @@
     </row>
     <row r="175" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="B175" t="s">
         <v>48</v>
@@ -17530,7 +17530,7 @@
     </row>
     <row r="176" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B176" t="s">
         <v>48</v>
@@ -17622,7 +17622,7 @@
     </row>
     <row r="177" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="B177" t="s">
         <v>48</v>
@@ -17714,7 +17714,7 @@
     </row>
     <row r="178" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="B178" t="s">
         <v>48</v>
@@ -17806,7 +17806,7 @@
     </row>
     <row r="179" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="B179" t="s">
         <v>45</v>
@@ -17910,7 +17910,7 @@
     </row>
     <row r="180" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="B180" t="s">
         <v>48</v>
@@ -18002,7 +18002,7 @@
     </row>
     <row r="181" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="B181" t="s">
         <v>48</v>
@@ -18094,7 +18094,7 @@
     </row>
     <row r="182" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="B182" t="s">
         <v>48</v>
@@ -18186,7 +18186,7 @@
     </row>
     <row r="183" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="B183" t="s">
         <v>48</v>
@@ -18278,7 +18278,7 @@
     </row>
     <row r="184" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="B184" t="s">
         <v>48</v>
@@ -18370,7 +18370,7 @@
     </row>
     <row r="185" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="B185" t="s">
         <v>48</v>

</xml_diff>